<commit_message>
preparing data for testing
</commit_message>
<xml_diff>
--- a/PN_demographics_neiu.xlsx
+++ b/PN_demographics_neiu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\Documents\Tutoring\CLASSES\MASTERS_PROJECT\code\m_project_code\topic-model-creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA0A1A4-25BF-4148-9330-8879C4D6486C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D1291-BF63-46EA-A265-322C7CCC12CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="1332" windowWidth="22116" windowHeight="10836" xr2:uid="{24881F79-2993-4647-9C59-9127DC6ADD26}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24881F79-2993-4647-9C59-9127DC6ADD26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5128" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5127" uniqueCount="265">
   <si>
     <t>record_id</t>
   </si>
@@ -336,9 +336,6 @@
   </si>
   <si>
     <t>toishanese</t>
-  </si>
-  <si>
-    <t>guangdon</t>
   </si>
   <si>
     <t xml:space="preserve">guangdon </t>
@@ -1184,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1F03B-AD1E-4BA1-970D-506D1D3B48D2}">
   <dimension ref="A1:L736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5602,14 +5599,11 @@
       <c r="F118" t="s">
         <v>15</v>
       </c>
-      <c r="G118" t="s">
-        <v>101</v>
-      </c>
       <c r="H118" t="s">
         <v>19</v>
       </c>
       <c r="I118" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J118">
         <v>60616</v>
@@ -5647,7 +5641,7 @@
         <v>30</v>
       </c>
       <c r="I119" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J119">
         <v>60616</v>
@@ -5761,7 +5755,7 @@
         <v>16</v>
       </c>
       <c r="I122" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J122">
         <v>60616</v>
@@ -5808,7 +5802,7 @@
         <v>5</v>
       </c>
       <c r="L123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
@@ -5837,7 +5831,7 @@
         <v>91</v>
       </c>
       <c r="I124" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J124">
         <v>60616</v>
@@ -5875,7 +5869,7 @@
         <v>16</v>
       </c>
       <c r="I125" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J125">
         <v>60616</v>
@@ -5913,7 +5907,7 @@
         <v>16</v>
       </c>
       <c r="I126" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J126">
         <v>60609</v>
@@ -5951,7 +5945,7 @@
         <v>19</v>
       </c>
       <c r="I127" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J127">
         <v>60616</v>
@@ -5989,7 +5983,7 @@
         <v>30</v>
       </c>
       <c r="I128" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J128">
         <v>60616</v>
@@ -6027,7 +6021,7 @@
         <v>19</v>
       </c>
       <c r="I129" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J129">
         <v>60632</v>
@@ -6065,7 +6059,7 @@
         <v>19</v>
       </c>
       <c r="I130" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J130">
         <v>60616</v>
@@ -6103,7 +6097,7 @@
         <v>30</v>
       </c>
       <c r="I131" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J131">
         <v>60608</v>
@@ -6138,7 +6132,7 @@
         <v>16</v>
       </c>
       <c r="I132" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J132">
         <v>60616</v>
@@ -6252,7 +6246,7 @@
         <v>16</v>
       </c>
       <c r="I135" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J135">
         <v>60608</v>
@@ -6287,7 +6281,7 @@
         <v>16</v>
       </c>
       <c r="I136" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J136">
         <v>60616</v>
@@ -6313,7 +6307,7 @@
         <v>13</v>
       </c>
       <c r="E137" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F137" t="s">
         <v>15</v>
@@ -6363,7 +6357,7 @@
         <v>16</v>
       </c>
       <c r="I138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J138">
         <v>60609</v>
@@ -6401,7 +6395,7 @@
         <v>16</v>
       </c>
       <c r="I139" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J139">
         <v>60632</v>
@@ -6439,7 +6433,7 @@
         <v>16</v>
       </c>
       <c r="I140" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J140">
         <v>60605</v>
@@ -6477,7 +6471,7 @@
         <v>19</v>
       </c>
       <c r="I141" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J141">
         <v>60609</v>
@@ -6515,7 +6509,7 @@
         <v>19</v>
       </c>
       <c r="I142" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J142">
         <v>60632</v>
@@ -6734,7 +6728,7 @@
         <v>30</v>
       </c>
       <c r="I148" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J148">
         <v>60609</v>
@@ -6810,7 +6804,7 @@
         <v>16</v>
       </c>
       <c r="I150" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J150">
         <v>60616</v>
@@ -6895,7 +6889,7 @@
         <v>2</v>
       </c>
       <c r="L152" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
@@ -6997,7 +6991,7 @@
         <v>16</v>
       </c>
       <c r="I155" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J155">
         <v>60609</v>
@@ -7035,7 +7029,7 @@
         <v>16</v>
       </c>
       <c r="I156" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J156">
         <v>60616</v>
@@ -7301,7 +7295,7 @@
         <v>30</v>
       </c>
       <c r="I163" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J163">
         <v>60616</v>
@@ -7362,7 +7356,7 @@
         <v>21</v>
       </c>
       <c r="D165" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E165" t="s">
         <v>22</v>
@@ -7377,7 +7371,7 @@
         <v>16</v>
       </c>
       <c r="I165" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J165">
         <v>60608</v>
@@ -7453,7 +7447,7 @@
         <v>16</v>
       </c>
       <c r="I167" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J167">
         <v>60616</v>
@@ -7491,7 +7485,7 @@
         <v>16</v>
       </c>
       <c r="I168" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J168">
         <v>60608</v>
@@ -7529,7 +7523,7 @@
         <v>16</v>
       </c>
       <c r="I169" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J169">
         <v>60616</v>
@@ -7567,7 +7561,7 @@
         <v>19</v>
       </c>
       <c r="I170" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J170">
         <v>60616</v>
@@ -7605,7 +7599,7 @@
         <v>30</v>
       </c>
       <c r="I171" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J171">
         <v>60632</v>
@@ -7681,7 +7675,7 @@
         <v>16</v>
       </c>
       <c r="I173" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J173">
         <v>60632</v>
@@ -7719,7 +7713,7 @@
         <v>30</v>
       </c>
       <c r="I174" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J174">
         <v>60608</v>
@@ -7795,7 +7789,7 @@
         <v>19</v>
       </c>
       <c r="I176" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J176">
         <v>60609</v>
@@ -7833,7 +7827,7 @@
         <v>19</v>
       </c>
       <c r="I177" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J177">
         <v>60632</v>
@@ -7985,7 +7979,7 @@
         <v>16</v>
       </c>
       <c r="I181" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J181">
         <v>60609</v>
@@ -8023,7 +8017,7 @@
         <v>16</v>
       </c>
       <c r="I182" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J182">
         <v>60616</v>
@@ -8175,7 +8169,7 @@
         <v>30</v>
       </c>
       <c r="I186" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J186">
         <v>60616</v>
@@ -8213,7 +8207,7 @@
         <v>19</v>
       </c>
       <c r="I187" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J187">
         <v>60605</v>
@@ -8289,7 +8283,7 @@
         <v>16</v>
       </c>
       <c r="I189" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J189">
         <v>60616</v>
@@ -8403,7 +8397,7 @@
         <v>16</v>
       </c>
       <c r="I192" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J192">
         <v>60616</v>
@@ -8660,7 +8654,7 @@
         <v>16</v>
       </c>
       <c r="I199" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J199">
         <v>60616</v>
@@ -8736,7 +8730,7 @@
         <v>16</v>
       </c>
       <c r="I201" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J201">
         <v>60616</v>
@@ -8812,7 +8806,7 @@
         <v>16</v>
       </c>
       <c r="I203" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J203">
         <v>60609</v>
@@ -8850,7 +8844,7 @@
         <v>16</v>
       </c>
       <c r="I204" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J204">
         <v>60616</v>
@@ -8999,7 +8993,7 @@
         <v>30</v>
       </c>
       <c r="I208" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J208">
         <v>60632</v>
@@ -9037,7 +9031,7 @@
         <v>16</v>
       </c>
       <c r="I209" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J209">
         <v>60632</v>
@@ -9075,7 +9069,7 @@
         <v>16</v>
       </c>
       <c r="I210" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J210">
         <v>60608</v>
@@ -9224,7 +9218,7 @@
         <v>19</v>
       </c>
       <c r="I214" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J214">
         <v>60616</v>
@@ -9262,7 +9256,7 @@
         <v>16</v>
       </c>
       <c r="I215" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J215">
         <v>60632</v>
@@ -9367,7 +9361,7 @@
         <v>22</v>
       </c>
       <c r="F218" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G218">
         <v>1981</v>
@@ -9376,7 +9370,7 @@
         <v>16</v>
       </c>
       <c r="I218" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J218">
         <v>60605</v>
@@ -9414,7 +9408,7 @@
         <v>19</v>
       </c>
       <c r="I219" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J219">
         <v>60616</v>
@@ -9452,7 +9446,7 @@
         <v>19</v>
       </c>
       <c r="I220" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J220">
         <v>60616</v>
@@ -9528,7 +9522,7 @@
         <v>30</v>
       </c>
       <c r="I222" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J222">
         <v>60616</v>
@@ -9566,7 +9560,7 @@
         <v>19</v>
       </c>
       <c r="I223" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J223">
         <v>60616</v>
@@ -9604,7 +9598,7 @@
         <v>19</v>
       </c>
       <c r="I224" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J224">
         <v>60616</v>
@@ -9756,7 +9750,7 @@
         <v>30</v>
       </c>
       <c r="I228" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J228">
         <v>60616</v>
@@ -9946,7 +9940,7 @@
         <v>16</v>
       </c>
       <c r="I233" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J233">
         <v>60616</v>
@@ -9984,7 +9978,7 @@
         <v>19</v>
       </c>
       <c r="I234" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J234">
         <v>60616</v>
@@ -10136,7 +10130,7 @@
         <v>19</v>
       </c>
       <c r="I238" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J238">
         <v>60616</v>
@@ -10174,7 +10168,7 @@
         <v>19</v>
       </c>
       <c r="I239" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J239">
         <v>60616</v>
@@ -10212,7 +10206,7 @@
         <v>19</v>
       </c>
       <c r="I240" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J240">
         <v>60616</v>
@@ -10249,11 +10243,11 @@
       <c r="H241" t="s">
         <v>16</v>
       </c>
-      <c r="I241">
-        <v>60616</v>
-      </c>
-      <c r="J241" t="s">
+      <c r="I241" t="s">
         <v>73</v>
+      </c>
+      <c r="J241">
+        <v>60616</v>
       </c>
       <c r="K241">
         <v>2</v>
@@ -10402,7 +10396,7 @@
         <v>19</v>
       </c>
       <c r="I245" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J245">
         <v>60616</v>
@@ -10507,7 +10501,7 @@
         <v>16</v>
       </c>
       <c r="I248" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J248">
         <v>60616</v>
@@ -10580,7 +10574,7 @@
         <v>30</v>
       </c>
       <c r="I250" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J250">
         <v>60616</v>
@@ -10694,7 +10688,7 @@
         <v>30</v>
       </c>
       <c r="I253" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J253">
         <v>60616</v>
@@ -10755,7 +10749,7 @@
         <v>12</v>
       </c>
       <c r="D255" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E255" t="s">
         <v>47</v>
@@ -10770,7 +10764,7 @@
         <v>19</v>
       </c>
       <c r="I255" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J255">
         <v>60616</v>
@@ -10805,7 +10799,7 @@
         <v>16</v>
       </c>
       <c r="I256" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J256">
         <v>60632</v>
@@ -10957,7 +10951,7 @@
         <v>91</v>
       </c>
       <c r="I260" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J260">
         <v>60608</v>
@@ -11065,7 +11059,7 @@
         <v>16</v>
       </c>
       <c r="I263" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J263">
         <v>60608</v>
@@ -11217,7 +11211,7 @@
         <v>19</v>
       </c>
       <c r="I267" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J267">
         <v>60605</v>
@@ -11255,7 +11249,7 @@
         <v>19</v>
       </c>
       <c r="I268" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J268">
         <v>60605</v>
@@ -11331,7 +11325,7 @@
         <v>30</v>
       </c>
       <c r="I270" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J270">
         <v>60616</v>
@@ -11340,7 +11334,7 @@
         <v>2</v>
       </c>
       <c r="L270" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.3">
@@ -11547,7 +11541,7 @@
         <v>16</v>
       </c>
       <c r="I276" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J276">
         <v>60616</v>
@@ -11578,14 +11572,11 @@
       <c r="F277" t="s">
         <v>15</v>
       </c>
-      <c r="G277">
-        <v>60608</v>
-      </c>
       <c r="H277" t="s">
         <v>19</v>
       </c>
       <c r="I277" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J277">
         <v>60616</v>
@@ -11962,7 +11953,7 @@
         <v>19</v>
       </c>
       <c r="I287" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J287">
         <v>60616</v>
@@ -12000,7 +11991,7 @@
         <v>16</v>
       </c>
       <c r="I288" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J288">
         <v>60608</v>
@@ -12038,7 +12029,7 @@
         <v>19</v>
       </c>
       <c r="I289" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J289">
         <v>60632</v>
@@ -12114,7 +12105,7 @@
         <v>16</v>
       </c>
       <c r="I291" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J291">
         <v>60608</v>
@@ -12213,7 +12204,7 @@
         <v>21</v>
       </c>
       <c r="D294" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E294" t="s">
         <v>47</v>
@@ -12228,7 +12219,7 @@
         <v>16</v>
       </c>
       <c r="I294" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J294">
         <v>60608</v>
@@ -12266,7 +12257,7 @@
         <v>19</v>
       </c>
       <c r="I295" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J295">
         <v>60616</v>
@@ -12304,7 +12295,7 @@
         <v>16</v>
       </c>
       <c r="I296" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J296">
         <v>60616</v>
@@ -12456,7 +12447,7 @@
         <v>30</v>
       </c>
       <c r="I300" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J300">
         <v>60608</v>
@@ -12494,7 +12485,7 @@
         <v>16</v>
       </c>
       <c r="I301" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J301">
         <v>60616</v>
@@ -12684,7 +12675,7 @@
         <v>30</v>
       </c>
       <c r="I306" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J306">
         <v>60616</v>
@@ -12760,7 +12751,7 @@
         <v>16</v>
       </c>
       <c r="I308" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J308">
         <v>60608</v>
@@ -12783,7 +12774,7 @@
         <v>21</v>
       </c>
       <c r="D309" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E309" t="s">
         <v>14</v>
@@ -12950,7 +12941,7 @@
         <v>19</v>
       </c>
       <c r="I313" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J313">
         <v>60616</v>
@@ -12988,7 +12979,7 @@
         <v>19</v>
       </c>
       <c r="I314" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J314">
         <v>60609</v>
@@ -13178,7 +13169,7 @@
         <v>19</v>
       </c>
       <c r="I319" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J319">
         <v>60608</v>
@@ -13236,7 +13227,7 @@
         <v>51</v>
       </c>
       <c r="D321" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E321" t="s">
         <v>22</v>
@@ -13327,7 +13318,7 @@
         <v>19</v>
       </c>
       <c r="I323" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J323">
         <v>60632</v>
@@ -13365,7 +13356,7 @@
         <v>16</v>
       </c>
       <c r="I324" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J324">
         <v>60616</v>
@@ -13403,7 +13394,7 @@
         <v>19</v>
       </c>
       <c r="I325" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J325">
         <v>60616</v>
@@ -13479,7 +13470,7 @@
         <v>16</v>
       </c>
       <c r="I327" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J327">
         <v>60609</v>
@@ -13669,7 +13660,7 @@
         <v>16</v>
       </c>
       <c r="I332" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J332">
         <v>60632</v>
@@ -13783,7 +13774,7 @@
         <v>19</v>
       </c>
       <c r="I335" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J335">
         <v>60616</v>
@@ -13821,7 +13812,7 @@
         <v>16</v>
       </c>
       <c r="I336" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J336">
         <v>60608</v>
@@ -13856,7 +13847,7 @@
         <v>19</v>
       </c>
       <c r="I337" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J337">
         <v>60616</v>
@@ -14046,7 +14037,7 @@
         <v>16</v>
       </c>
       <c r="I342" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J342">
         <v>60632</v>
@@ -14122,7 +14113,7 @@
         <v>19</v>
       </c>
       <c r="I344" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J344">
         <v>60608</v>
@@ -14160,7 +14151,7 @@
         <v>16</v>
       </c>
       <c r="I345" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J345">
         <v>60632</v>
@@ -14236,7 +14227,7 @@
         <v>19</v>
       </c>
       <c r="I347" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J347">
         <v>60616</v>
@@ -14388,7 +14379,7 @@
         <v>16</v>
       </c>
       <c r="I351" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J351">
         <v>60616</v>
@@ -14426,7 +14417,7 @@
         <v>16</v>
       </c>
       <c r="I352" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J352">
         <v>60632</v>
@@ -14540,7 +14531,7 @@
         <v>30</v>
       </c>
       <c r="I355" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J355">
         <v>60616</v>
@@ -14756,7 +14747,7 @@
         <v>62</v>
       </c>
       <c r="E361" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F361" t="s">
         <v>15</v>
@@ -14768,7 +14759,7 @@
         <v>30</v>
       </c>
       <c r="I361" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J361">
         <v>60608</v>
@@ -14920,7 +14911,7 @@
         <v>19</v>
       </c>
       <c r="I365" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J365">
         <v>60616</v>
@@ -15180,7 +15171,7 @@
         <v>30</v>
       </c>
       <c r="I372" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J372">
         <v>60616</v>
@@ -15218,7 +15209,7 @@
         <v>30</v>
       </c>
       <c r="I373" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J373">
         <v>60616</v>
@@ -15256,7 +15247,7 @@
         <v>19</v>
       </c>
       <c r="I374" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J374">
         <v>60632</v>
@@ -15332,7 +15323,7 @@
         <v>16</v>
       </c>
       <c r="I376" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J376">
         <v>60616</v>
@@ -15481,7 +15472,7 @@
         <v>16</v>
       </c>
       <c r="I380" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J380">
         <v>60616</v>
@@ -15519,7 +15510,7 @@
         <v>16</v>
       </c>
       <c r="I381" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J381">
         <v>60616</v>
@@ -15709,7 +15700,7 @@
         <v>19</v>
       </c>
       <c r="I386" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J386">
         <v>60616</v>
@@ -15747,7 +15738,7 @@
         <v>30</v>
       </c>
       <c r="I387" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J387">
         <v>60608</v>
@@ -15861,7 +15852,7 @@
         <v>16</v>
       </c>
       <c r="I390" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J390">
         <v>60616</v>
@@ -15937,7 +15928,7 @@
         <v>16</v>
       </c>
       <c r="I392" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J392">
         <v>60616</v>
@@ -15998,7 +15989,7 @@
         <v>21</v>
       </c>
       <c r="D394" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E394" t="s">
         <v>14</v>
@@ -16159,7 +16150,7 @@
         <v>15</v>
       </c>
       <c r="G398">
-        <v>96</v>
+        <v>1996</v>
       </c>
       <c r="H398" t="s">
         <v>16</v>
@@ -16317,7 +16308,7 @@
         <v>19</v>
       </c>
       <c r="I402" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J402">
         <v>60616</v>
@@ -16469,7 +16460,7 @@
         <v>16</v>
       </c>
       <c r="I406" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J406">
         <v>60616</v>
@@ -16621,7 +16612,7 @@
         <v>19</v>
       </c>
       <c r="I410" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J410">
         <v>60632</v>
@@ -16653,7 +16644,7 @@
         <v>15</v>
       </c>
       <c r="G411">
-        <v>6</v>
+        <v>2006</v>
       </c>
       <c r="H411" t="s">
         <v>19</v>
@@ -16697,7 +16688,7 @@
         <v>19</v>
       </c>
       <c r="I412" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J412">
         <v>60616</v>
@@ -16811,7 +16802,7 @@
         <v>16</v>
       </c>
       <c r="I415" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J415">
         <v>60616</v>
@@ -16887,7 +16878,7 @@
         <v>30</v>
       </c>
       <c r="I417" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J417">
         <v>60609</v>
@@ -16925,7 +16916,7 @@
         <v>19</v>
       </c>
       <c r="I418" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J418">
         <v>60616</v>
@@ -16963,7 +16954,7 @@
         <v>16</v>
       </c>
       <c r="I419" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J419">
         <v>60616</v>
@@ -17077,7 +17068,7 @@
         <v>16</v>
       </c>
       <c r="I422" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J422">
         <v>60632</v>
@@ -17153,7 +17144,7 @@
         <v>19</v>
       </c>
       <c r="I424" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J424">
         <v>60616</v>
@@ -17191,7 +17182,7 @@
         <v>16</v>
       </c>
       <c r="I425" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J425">
         <v>60616</v>
@@ -17267,7 +17258,7 @@
         <v>30</v>
       </c>
       <c r="I427" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J427">
         <v>60609</v>
@@ -17495,7 +17486,7 @@
         <v>19</v>
       </c>
       <c r="I433" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J433">
         <v>60608</v>
@@ -17609,7 +17600,7 @@
         <v>30</v>
       </c>
       <c r="I436" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J436">
         <v>60616</v>
@@ -17647,7 +17638,7 @@
         <v>16</v>
       </c>
       <c r="I437" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J437">
         <v>60616</v>
@@ -17761,7 +17752,7 @@
         <v>16</v>
       </c>
       <c r="I440" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J440">
         <v>60616</v>
@@ -17799,7 +17790,7 @@
         <v>30</v>
       </c>
       <c r="I441" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J441">
         <v>60608</v>
@@ -17846,7 +17837,7 @@
         <v>5</v>
       </c>
       <c r="L442" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="443" spans="1:12" x14ac:dyDescent="0.3">
@@ -17875,7 +17866,7 @@
         <v>30</v>
       </c>
       <c r="I443" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J443">
         <v>60616</v>
@@ -17913,7 +17904,7 @@
         <v>16</v>
       </c>
       <c r="I444" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J444">
         <v>60616</v>
@@ -17954,7 +17945,7 @@
         <v>97</v>
       </c>
       <c r="J445">
-        <v>6069</v>
+        <v>60609</v>
       </c>
       <c r="K445">
         <v>4</v>
@@ -18027,7 +18018,7 @@
         <v>16</v>
       </c>
       <c r="I447" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J447">
         <v>60609</v>
@@ -18103,7 +18094,7 @@
         <v>19</v>
       </c>
       <c r="I449" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J449">
         <v>60616</v>
@@ -18141,7 +18132,7 @@
         <v>19</v>
       </c>
       <c r="I450" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J450">
         <v>60632</v>
@@ -18179,7 +18170,7 @@
         <v>30</v>
       </c>
       <c r="I451" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J451">
         <v>60616</v>
@@ -18211,7 +18202,7 @@
         <v>15</v>
       </c>
       <c r="G452">
-        <v>94</v>
+        <v>1994</v>
       </c>
       <c r="H452" t="s">
         <v>30</v>
@@ -18255,7 +18246,7 @@
         <v>16</v>
       </c>
       <c r="I453" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J453">
         <v>60608</v>
@@ -18293,7 +18284,7 @@
         <v>30</v>
       </c>
       <c r="I454" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J454">
         <v>60608</v>
@@ -18369,7 +18360,7 @@
         <v>30</v>
       </c>
       <c r="I456" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J456">
         <v>60608</v>
@@ -18430,7 +18421,7 @@
         <v>33</v>
       </c>
       <c r="D458" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E458" t="s">
         <v>47</v>
@@ -18445,7 +18436,7 @@
         <v>16</v>
       </c>
       <c r="I458" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J458">
         <v>60616</v>
@@ -18477,7 +18468,7 @@
         <v>15</v>
       </c>
       <c r="G459">
-        <v>7</v>
+        <v>2007</v>
       </c>
       <c r="H459" t="s">
         <v>19</v>
@@ -18521,7 +18512,7 @@
         <v>16</v>
       </c>
       <c r="I460" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J460">
         <v>60609</v>
@@ -18559,7 +18550,7 @@
         <v>30</v>
       </c>
       <c r="I461" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J461">
         <v>60616</v>
@@ -18597,7 +18588,7 @@
         <v>30</v>
       </c>
       <c r="I462" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J462">
         <v>60616</v>
@@ -18635,7 +18626,7 @@
         <v>19</v>
       </c>
       <c r="I463" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J463">
         <v>60609</v>
@@ -18711,7 +18702,7 @@
         <v>16</v>
       </c>
       <c r="I465" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J465">
         <v>60608</v>
@@ -18825,7 +18816,7 @@
         <v>16</v>
       </c>
       <c r="I468" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J468">
         <v>60616</v>
@@ -18863,7 +18854,7 @@
         <v>19</v>
       </c>
       <c r="I469" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J469">
         <v>60608</v>
@@ -19053,7 +19044,7 @@
         <v>19</v>
       </c>
       <c r="I474" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J474">
         <v>60616</v>
@@ -19091,7 +19082,7 @@
         <v>19</v>
       </c>
       <c r="I475" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J475">
         <v>60632</v>
@@ -19100,7 +19091,7 @@
         <v>2</v>
       </c>
       <c r="L475" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="476" spans="1:12" x14ac:dyDescent="0.3">
@@ -19167,7 +19158,7 @@
         <v>19</v>
       </c>
       <c r="I477" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J477">
         <v>60608</v>
@@ -19243,7 +19234,7 @@
         <v>19</v>
       </c>
       <c r="I479" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J479">
         <v>60616</v>
@@ -19357,7 +19348,7 @@
         <v>19</v>
       </c>
       <c r="I482" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J482">
         <v>60616</v>
@@ -19404,7 +19395,7 @@
         <v>7</v>
       </c>
       <c r="L483" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="484" spans="1:12" x14ac:dyDescent="0.3">
@@ -19471,7 +19462,7 @@
         <v>19</v>
       </c>
       <c r="I485" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J485">
         <v>60616</v>
@@ -19509,7 +19500,7 @@
         <v>19</v>
       </c>
       <c r="I486" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J486">
         <v>60616</v>
@@ -19585,7 +19576,7 @@
         <v>16</v>
       </c>
       <c r="I488" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J488">
         <v>60609</v>
@@ -19623,7 +19614,7 @@
         <v>30</v>
       </c>
       <c r="I489" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J489">
         <v>60616</v>
@@ -19661,7 +19652,7 @@
         <v>16</v>
       </c>
       <c r="I490" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J490">
         <v>60616</v>
@@ -19737,7 +19728,7 @@
         <v>19</v>
       </c>
       <c r="I492" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J492">
         <v>60616</v>
@@ -19775,7 +19766,7 @@
         <v>16</v>
       </c>
       <c r="I493" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J493">
         <v>60616</v>
@@ -19813,7 +19804,7 @@
         <v>16</v>
       </c>
       <c r="I494" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J494">
         <v>60616</v>
@@ -19965,7 +19956,7 @@
         <v>19</v>
       </c>
       <c r="I498" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J498">
         <v>60632</v>
@@ -20079,7 +20070,7 @@
         <v>19</v>
       </c>
       <c r="I501" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J501">
         <v>60616</v>
@@ -20307,7 +20298,7 @@
         <v>91</v>
       </c>
       <c r="I507" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J507">
         <v>60616</v>
@@ -20345,7 +20336,7 @@
         <v>16</v>
       </c>
       <c r="I508" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J508">
         <v>60616</v>
@@ -20383,7 +20374,7 @@
         <v>16</v>
       </c>
       <c r="I509" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J509">
         <v>60616</v>
@@ -20459,7 +20450,7 @@
         <v>16</v>
       </c>
       <c r="I511" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J511">
         <v>60632</v>
@@ -20535,7 +20526,7 @@
         <v>19</v>
       </c>
       <c r="I513" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J513">
         <v>60608</v>
@@ -20573,7 +20564,7 @@
         <v>19</v>
       </c>
       <c r="I514" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J514">
         <v>60616</v>
@@ -20611,7 +20602,7 @@
         <v>19</v>
       </c>
       <c r="I515" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J515">
         <v>60616</v>
@@ -20687,7 +20678,7 @@
         <v>19</v>
       </c>
       <c r="I517" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J517">
         <v>60632</v>
@@ -20725,7 +20716,7 @@
         <v>19</v>
       </c>
       <c r="I518" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J518">
         <v>60609</v>
@@ -20877,7 +20868,7 @@
         <v>16</v>
       </c>
       <c r="I522" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J522">
         <v>60616</v>
@@ -20991,7 +20982,7 @@
         <v>16</v>
       </c>
       <c r="I525" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J525">
         <v>60623</v>
@@ -21067,7 +21058,7 @@
         <v>16</v>
       </c>
       <c r="I527" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J527">
         <v>60616</v>
@@ -21105,7 +21096,7 @@
         <v>19</v>
       </c>
       <c r="I528" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J528">
         <v>60616</v>
@@ -21152,7 +21143,7 @@
         <v>5</v>
       </c>
       <c r="L529" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="530" spans="1:12" x14ac:dyDescent="0.3">
@@ -21181,7 +21172,7 @@
         <v>19</v>
       </c>
       <c r="I530" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J530">
         <v>60616</v>
@@ -21219,7 +21210,7 @@
         <v>16</v>
       </c>
       <c r="I531" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J531">
         <v>60616</v>
@@ -21371,7 +21362,7 @@
         <v>19</v>
       </c>
       <c r="I535" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J535">
         <v>60616</v>
@@ -21394,7 +21385,7 @@
         <v>33</v>
       </c>
       <c r="D536" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E536" t="s">
         <v>47</v>
@@ -21418,7 +21409,7 @@
         <v>3</v>
       </c>
       <c r="L536" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="537" spans="1:12" x14ac:dyDescent="0.3">
@@ -21485,7 +21476,7 @@
         <v>19</v>
       </c>
       <c r="I538" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J538">
         <v>60616</v>
@@ -21561,7 +21552,7 @@
         <v>30</v>
       </c>
       <c r="I540" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J540">
         <v>60608</v>
@@ -21713,7 +21704,7 @@
         <v>16</v>
       </c>
       <c r="I544" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J544">
         <v>60608</v>
@@ -21751,7 +21742,7 @@
         <v>16</v>
       </c>
       <c r="I545" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J545">
         <v>60609</v>
@@ -21827,7 +21818,7 @@
         <v>16</v>
       </c>
       <c r="I547" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J547">
         <v>60616</v>
@@ -21865,7 +21856,7 @@
         <v>16</v>
       </c>
       <c r="I548" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J548">
         <v>60608</v>
@@ -21988,7 +21979,7 @@
         <v>5</v>
       </c>
       <c r="L551" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="552" spans="1:12" x14ac:dyDescent="0.3">
@@ -22131,7 +22122,7 @@
         <v>30</v>
       </c>
       <c r="I555" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J555">
         <v>60609</v>
@@ -22169,7 +22160,7 @@
         <v>16</v>
       </c>
       <c r="I556" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J556">
         <v>60616</v>
@@ -22207,7 +22198,7 @@
         <v>30</v>
       </c>
       <c r="I557" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J557">
         <v>60616</v>
@@ -22283,7 +22274,7 @@
         <v>16</v>
       </c>
       <c r="I559" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J559">
         <v>60616</v>
@@ -22321,7 +22312,7 @@
         <v>19</v>
       </c>
       <c r="I560" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J560">
         <v>60616</v>
@@ -22359,7 +22350,7 @@
         <v>19</v>
       </c>
       <c r="I561" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J561">
         <v>60616</v>
@@ -22406,7 +22397,7 @@
         <v>7</v>
       </c>
       <c r="L562" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="563" spans="1:12" x14ac:dyDescent="0.3">
@@ -22435,7 +22426,7 @@
         <v>19</v>
       </c>
       <c r="I563" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J563">
         <v>60608</v>
@@ -22473,7 +22464,7 @@
         <v>19</v>
       </c>
       <c r="I564" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J564">
         <v>60616</v>
@@ -22511,7 +22502,7 @@
         <v>16</v>
       </c>
       <c r="I565" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J565">
         <v>60616</v>
@@ -22587,7 +22578,7 @@
         <v>16</v>
       </c>
       <c r="I567" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J567">
         <v>60608</v>
@@ -22663,7 +22654,7 @@
         <v>19</v>
       </c>
       <c r="I569" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J569">
         <v>60616</v>
@@ -22701,7 +22692,7 @@
         <v>16</v>
       </c>
       <c r="I570" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J570">
         <v>60616</v>
@@ -22748,7 +22739,7 @@
         <v>5</v>
       </c>
       <c r="L571" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="572" spans="1:12" x14ac:dyDescent="0.3">
@@ -22777,7 +22768,7 @@
         <v>16</v>
       </c>
       <c r="I572" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J572">
         <v>60616</v>
@@ -22815,7 +22806,7 @@
         <v>16</v>
       </c>
       <c r="I573" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J573">
         <v>60616</v>
@@ -22891,7 +22882,7 @@
         <v>30</v>
       </c>
       <c r="I575" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J575">
         <v>60608</v>
@@ -23081,7 +23072,7 @@
         <v>16</v>
       </c>
       <c r="I580" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J580">
         <v>60608</v>
@@ -23195,7 +23186,7 @@
         <v>16</v>
       </c>
       <c r="I583" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J583">
         <v>60609</v>
@@ -23347,7 +23338,7 @@
         <v>16</v>
       </c>
       <c r="I587" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J587">
         <v>60608</v>
@@ -23423,7 +23414,7 @@
         <v>19</v>
       </c>
       <c r="I589" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J589">
         <v>60608</v>
@@ -23461,7 +23452,7 @@
         <v>19</v>
       </c>
       <c r="I590" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J590">
         <v>60608</v>
@@ -23499,7 +23490,7 @@
         <v>16</v>
       </c>
       <c r="I591" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J591">
         <v>60608</v>
@@ -23537,7 +23528,7 @@
         <v>30</v>
       </c>
       <c r="I592" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J592">
         <v>60608</v>
@@ -23575,7 +23566,7 @@
         <v>16</v>
       </c>
       <c r="I593" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J593">
         <v>60616</v>
@@ -23651,7 +23642,7 @@
         <v>30</v>
       </c>
       <c r="I595" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J595">
         <v>60608</v>
@@ -23689,7 +23680,7 @@
         <v>19</v>
       </c>
       <c r="I596" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J596">
         <v>60608</v>
@@ -23727,7 +23718,7 @@
         <v>19</v>
       </c>
       <c r="I597" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J597">
         <v>60616</v>
@@ -23803,7 +23794,7 @@
         <v>16</v>
       </c>
       <c r="I599" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J599">
         <v>60616</v>
@@ -23879,7 +23870,7 @@
         <v>16</v>
       </c>
       <c r="I601" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J601">
         <v>60616</v>
@@ -23993,7 +23984,7 @@
         <v>16</v>
       </c>
       <c r="I604" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J604">
         <v>60609</v>
@@ -24031,7 +24022,7 @@
         <v>19</v>
       </c>
       <c r="I605" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J605">
         <v>60608</v>
@@ -24183,7 +24174,7 @@
         <v>30</v>
       </c>
       <c r="I609" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J609">
         <v>60616</v>
@@ -24297,7 +24288,7 @@
         <v>19</v>
       </c>
       <c r="I612" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J612">
         <v>60616</v>
@@ -24320,7 +24311,7 @@
         <v>21</v>
       </c>
       <c r="D613" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E613" t="s">
         <v>45</v>
@@ -24335,7 +24326,7 @@
         <v>30</v>
       </c>
       <c r="I613" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J613">
         <v>60616</v>
@@ -24373,7 +24364,7 @@
         <v>16</v>
       </c>
       <c r="I614" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J614">
         <v>60616</v>
@@ -24487,7 +24478,7 @@
         <v>16</v>
       </c>
       <c r="I617" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J617">
         <v>60616</v>
@@ -24525,7 +24516,7 @@
         <v>16</v>
       </c>
       <c r="I618" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J618">
         <v>60616</v>
@@ -24563,7 +24554,7 @@
         <v>16</v>
       </c>
       <c r="I619" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J619">
         <v>60616</v>
@@ -24595,13 +24586,13 @@
         <v>15</v>
       </c>
       <c r="G620">
-        <v>18</v>
+        <v>2018</v>
       </c>
       <c r="H620" t="s">
         <v>16</v>
       </c>
       <c r="I620" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J620">
         <v>60616</v>
@@ -24639,7 +24630,7 @@
         <v>16</v>
       </c>
       <c r="I621" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J621">
         <v>60616</v>
@@ -24671,13 +24662,13 @@
         <v>15</v>
       </c>
       <c r="G622">
-        <v>12</v>
+        <v>2012</v>
       </c>
       <c r="H622" t="s">
         <v>19</v>
       </c>
       <c r="I622" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J622">
         <v>60616</v>
@@ -24753,7 +24744,7 @@
         <v>19</v>
       </c>
       <c r="I624" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J624">
         <v>60616</v>
@@ -24791,7 +24782,7 @@
         <v>16</v>
       </c>
       <c r="I625" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J625">
         <v>60609</v>
@@ -24829,7 +24820,7 @@
         <v>19</v>
       </c>
       <c r="I626" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J626">
         <v>60609</v>
@@ -24867,7 +24858,7 @@
         <v>16</v>
       </c>
       <c r="I627" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J627">
         <v>60632</v>
@@ -24943,7 +24934,7 @@
         <v>16</v>
       </c>
       <c r="I629" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J629">
         <v>60616</v>
@@ -25019,7 +25010,7 @@
         <v>16</v>
       </c>
       <c r="I631" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J631">
         <v>60608</v>
@@ -25057,7 +25048,7 @@
         <v>16</v>
       </c>
       <c r="I632" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J632">
         <v>60608</v>
@@ -25080,7 +25071,7 @@
         <v>21</v>
       </c>
       <c r="D633" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E633" t="s">
         <v>22</v>
@@ -25095,7 +25086,7 @@
         <v>16</v>
       </c>
       <c r="I633" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J633">
         <v>60616</v>
@@ -25133,7 +25124,7 @@
         <v>16</v>
       </c>
       <c r="I634" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J634">
         <v>60608</v>
@@ -25209,7 +25200,7 @@
         <v>30</v>
       </c>
       <c r="I636" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J636">
         <v>60608</v>
@@ -25285,7 +25276,7 @@
         <v>16</v>
       </c>
       <c r="I638" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J638">
         <v>60609</v>
@@ -25361,7 +25352,7 @@
         <v>16</v>
       </c>
       <c r="I640" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J640">
         <v>60632</v>
@@ -25399,7 +25390,7 @@
         <v>16</v>
       </c>
       <c r="I641" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J641">
         <v>60616</v>
@@ -25437,7 +25428,7 @@
         <v>30</v>
       </c>
       <c r="I642" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J642">
         <v>60608</v>
@@ -25475,7 +25466,7 @@
         <v>16</v>
       </c>
       <c r="I643" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J643">
         <v>60608</v>
@@ -25513,7 +25504,7 @@
         <v>16</v>
       </c>
       <c r="I644" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J644">
         <v>60616</v>
@@ -25548,7 +25539,7 @@
         <v>16</v>
       </c>
       <c r="I645" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J645">
         <v>60608</v>
@@ -25586,7 +25577,7 @@
         <v>16</v>
       </c>
       <c r="I646" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J646">
         <v>60608</v>
@@ -25624,7 +25615,7 @@
         <v>19</v>
       </c>
       <c r="I647" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J647">
         <v>60608</v>
@@ -25662,7 +25653,7 @@
         <v>19</v>
       </c>
       <c r="I648" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J648">
         <v>60609</v>
@@ -25723,7 +25714,7 @@
         <v>21</v>
       </c>
       <c r="D650" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E650" t="s">
         <v>22</v>
@@ -25738,7 +25729,7 @@
         <v>30</v>
       </c>
       <c r="I650" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J650">
         <v>60616</v>
@@ -25776,7 +25767,7 @@
         <v>19</v>
       </c>
       <c r="I651" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J651">
         <v>60632</v>
@@ -25814,7 +25805,7 @@
         <v>19</v>
       </c>
       <c r="I652" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J652">
         <v>60616</v>
@@ -25852,7 +25843,7 @@
         <v>16</v>
       </c>
       <c r="I653" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J653">
         <v>60608</v>
@@ -25928,7 +25919,7 @@
         <v>16</v>
       </c>
       <c r="I655" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J655">
         <v>60616</v>
@@ -25966,7 +25957,7 @@
         <v>16</v>
       </c>
       <c r="I656" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J656">
         <v>60616</v>
@@ -26042,7 +26033,7 @@
         <v>19</v>
       </c>
       <c r="I658" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J658">
         <v>60608</v>
@@ -26080,7 +26071,7 @@
         <v>19</v>
       </c>
       <c r="I659" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J659">
         <v>60616</v>
@@ -26118,7 +26109,7 @@
         <v>16</v>
       </c>
       <c r="I660" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J660">
         <v>60616</v>
@@ -26156,7 +26147,7 @@
         <v>16</v>
       </c>
       <c r="I661" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J661">
         <v>60616</v>
@@ -26194,7 +26185,7 @@
         <v>19</v>
       </c>
       <c r="I662" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J662">
         <v>60616</v>
@@ -26232,7 +26223,7 @@
         <v>30</v>
       </c>
       <c r="I663" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J663">
         <v>60605</v>
@@ -26270,7 +26261,7 @@
         <v>16</v>
       </c>
       <c r="I664" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J664">
         <v>60632</v>
@@ -26308,7 +26299,7 @@
         <v>16</v>
       </c>
       <c r="I665" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J665">
         <v>60608</v>
@@ -26346,7 +26337,7 @@
         <v>19</v>
       </c>
       <c r="I666" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J666">
         <v>60608</v>
@@ -26384,7 +26375,7 @@
         <v>16</v>
       </c>
       <c r="I667" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J667">
         <v>60616</v>
@@ -26422,7 +26413,7 @@
         <v>16</v>
       </c>
       <c r="I668" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J668">
         <v>60605</v>
@@ -26498,7 +26489,7 @@
         <v>16</v>
       </c>
       <c r="I670" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J670">
         <v>60616</v>
@@ -26574,7 +26565,7 @@
         <v>19</v>
       </c>
       <c r="I672" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J672">
         <v>60609</v>
@@ -26583,7 +26574,7 @@
         <v>6</v>
       </c>
       <c r="L672" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="673" spans="1:12" x14ac:dyDescent="0.3">
@@ -26612,7 +26603,7 @@
         <v>30</v>
       </c>
       <c r="I673" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J673">
         <v>60616</v>
@@ -26688,7 +26679,7 @@
         <v>16</v>
       </c>
       <c r="I675" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J675">
         <v>60616</v>
@@ -26726,7 +26717,7 @@
         <v>16</v>
       </c>
       <c r="I676" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J676">
         <v>60616</v>
@@ -26764,7 +26755,7 @@
         <v>30</v>
       </c>
       <c r="I677" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J677">
         <v>60632</v>
@@ -26840,7 +26831,7 @@
         <v>30</v>
       </c>
       <c r="I679" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J679">
         <v>60608</v>
@@ -26878,7 +26869,7 @@
         <v>30</v>
       </c>
       <c r="I680" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J680">
         <v>60616</v>
@@ -26916,7 +26907,7 @@
         <v>19</v>
       </c>
       <c r="I681" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J681">
         <v>60608</v>
@@ -26954,7 +26945,7 @@
         <v>16</v>
       </c>
       <c r="I682" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J682">
         <v>60608</v>
@@ -26992,7 +26983,7 @@
         <v>19</v>
       </c>
       <c r="I683" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J683">
         <v>60616</v>
@@ -27030,7 +27021,7 @@
         <v>16</v>
       </c>
       <c r="I684" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J684">
         <v>60616</v>
@@ -27068,7 +27059,7 @@
         <v>16</v>
       </c>
       <c r="I685" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J685">
         <v>60616</v>
@@ -27091,7 +27082,7 @@
         <v>33</v>
       </c>
       <c r="D686" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E686" t="s">
         <v>34</v>
@@ -27141,7 +27132,7 @@
         <v>19</v>
       </c>
       <c r="I687" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J687">
         <v>60608</v>
@@ -27217,7 +27208,7 @@
         <v>30</v>
       </c>
       <c r="I689" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J689">
         <v>60616</v>
@@ -27255,7 +27246,7 @@
         <v>16</v>
       </c>
       <c r="I690" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J690">
         <v>60616</v>
@@ -27293,7 +27284,7 @@
         <v>19</v>
       </c>
       <c r="I691" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J691">
         <v>60616</v>
@@ -27369,7 +27360,7 @@
         <v>30</v>
       </c>
       <c r="I693" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J693">
         <v>60632</v>
@@ -27407,7 +27398,7 @@
         <v>16</v>
       </c>
       <c r="I694" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J694">
         <v>60616</v>
@@ -27483,7 +27474,7 @@
         <v>19</v>
       </c>
       <c r="I696" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J696">
         <v>60616</v>
@@ -27492,7 +27483,7 @@
         <v>2</v>
       </c>
       <c r="L696" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="697" spans="1:12" x14ac:dyDescent="0.3">
@@ -27521,7 +27512,7 @@
         <v>16</v>
       </c>
       <c r="I697" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J697">
         <v>60616</v>
@@ -27597,7 +27588,7 @@
         <v>19</v>
       </c>
       <c r="I699" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J699">
         <v>60616</v>
@@ -27635,7 +27626,7 @@
         <v>30</v>
       </c>
       <c r="I700" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J700">
         <v>60632</v>
@@ -27673,7 +27664,7 @@
         <v>19</v>
       </c>
       <c r="I701" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J701">
         <v>60616</v>
@@ -27749,7 +27740,7 @@
         <v>16</v>
       </c>
       <c r="I703" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J703">
         <v>60616</v>
@@ -27787,7 +27778,7 @@
         <v>16</v>
       </c>
       <c r="I704" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J704">
         <v>60605</v>
@@ -27965,7 +27956,7 @@
         <v>16</v>
       </c>
       <c r="I709" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J709">
         <v>60616</v>
@@ -28003,7 +27994,7 @@
         <v>16</v>
       </c>
       <c r="I710" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J710">
         <v>60616</v>
@@ -28079,7 +28070,7 @@
         <v>16</v>
       </c>
       <c r="I712" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J712">
         <v>60607</v>
@@ -28193,7 +28184,7 @@
         <v>91</v>
       </c>
       <c r="I715" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J715">
         <v>60609</v>
@@ -28307,7 +28298,7 @@
         <v>30</v>
       </c>
       <c r="I718" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J718">
         <v>60616</v>
@@ -28345,7 +28336,7 @@
         <v>16</v>
       </c>
       <c r="I719" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J719">
         <v>60616</v>
@@ -28383,7 +28374,7 @@
         <v>19</v>
       </c>
       <c r="I720" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J720">
         <v>60616</v>
@@ -28497,7 +28488,7 @@
         <v>19</v>
       </c>
       <c r="I723" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J723">
         <v>60616</v>
@@ -28573,7 +28564,7 @@
         <v>30</v>
       </c>
       <c r="I725" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J725">
         <v>60608</v>
@@ -28611,7 +28602,7 @@
         <v>16</v>
       </c>
       <c r="I726" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J726">
         <v>60616</v>
@@ -28649,7 +28640,7 @@
         <v>16</v>
       </c>
       <c r="I727" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J727">
         <v>60616</v>
@@ -28763,7 +28754,7 @@
         <v>16</v>
       </c>
       <c r="I730" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J730">
         <v>60660</v>
@@ -28801,7 +28792,7 @@
         <v>19</v>
       </c>
       <c r="I731" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J731">
         <v>60605</v>

</xml_diff>